<commit_message>
phân công lần 2
</commit_message>
<xml_diff>
--- a/PhanCong.xlsx
+++ b/PhanCong.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Công việc</t>
   </si>
@@ -87,31 +87,28 @@
     <t>tạo user control riêng cho phân đăng nhập nha, add vào trong folder user control của project, lúc cần chỉ kéo thả vào page thôi, dựa theo yêu cầu trong file của thầy phúc.</t>
   </si>
   <si>
-    <t>Next</t>
+    <t>Thứ 7 (19/11/2010)</t>
   </si>
   <si>
-    <t>mail xác nhận</t>
+    <t>gõ submit thì gửi mail tới người dùng xác nhận</t>
   </si>
   <si>
-    <t>capchar</t>
+    <t>Thứ 4 (24/11/2010)</t>
   </si>
   <si>
-    <t>post get, connect giữa các trang</t>
+    <t>đăng nhập, đăng kí nhà tuyển dụng và người tìm việc, truy suất dữ liệu</t>
   </si>
   <si>
-    <t>tìm resource các file ảnh quảng cáo</t>
+    <t>submit đăng kí-&gt; lưu csdl</t>
   </si>
   <si>
-    <t>rss + feed cho phần hiển thị tin tức</t>
+    <t>tìm cách lưu trữ xác nhận capchars đúng hay sai</t>
   </si>
   <si>
-    <t>button đăng kí</t>
+    <t>tìm source ảnh capchar (khoảng 20 tấm) + ảnh gif quảng cáo</t>
   </si>
   <si>
-    <t>có dữ liệu -&gt; đăng nhập</t>
-  </si>
-  <si>
-    <t>Thứ 7 (19/11/2010)</t>
+    <t>hiển thị tin tức nổi bật (rss,feed), FAQ</t>
   </si>
 </sst>
 </file>
@@ -354,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -400,6 +397,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -416,15 +441,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -742,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L434"/>
+  <dimension ref="A1:L435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -759,20 +775,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1">
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -788,22 +804,22 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:12" ht="36" customHeight="1">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="39.75" customHeight="1">
-      <c r="B5" s="28"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="32"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -845,10 +861,10 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="63">
-      <c r="A8" s="20">
+      <c r="A8" s="30">
         <v>1</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -860,13 +876,13 @@
       <c r="E8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>31</v>
+      <c r="F8" s="27" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="31.5">
-      <c r="A9" s="21"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="8" t="s">
         <v>5</v>
       </c>
@@ -876,11 +892,11 @@
       <c r="E9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:12" ht="31.5">
-      <c r="A10" s="21"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
@@ -890,11 +906,11 @@
       <c r="E10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:12" ht="63">
-      <c r="A11" s="21"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
@@ -904,11 +920,11 @@
       <c r="E11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1">
+      <c r="A12" s="32"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
@@ -916,139 +932,163 @@
         <v>21</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="1:12" ht="21" customHeight="1">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:12" ht="15.75">
       <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" ht="45" customHeight="1">
+      <c r="A15" s="24">
+        <v>2</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="33" customHeight="1">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="28"/>
+    </row>
+    <row r="17" spans="1:6" ht="39" customHeight="1">
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="28"/>
+    </row>
+    <row r="18" spans="1:6" ht="34.5" customHeight="1">
+      <c r="A18" s="25"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
+      <c r="E18" s="15"/>
+      <c r="F18" s="28"/>
+    </row>
+    <row r="19" spans="1:6" ht="47.25" customHeight="1">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75">
+      <c r="E19" s="12"/>
+      <c r="F19" s="29"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75">
+    <row r="21" spans="1:6" ht="15.75">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75">
+    <row r="22" spans="1:6" ht="15.75">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75">
+    <row r="23" spans="1:6" ht="15.75">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75">
+    <row r="24" spans="1:6" ht="15.75">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75">
+    <row r="25" spans="1:6" ht="15.75">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75">
+    <row r="26" spans="1:6" ht="15.75">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75">
+    <row r="27" spans="1:6" ht="15.75">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75">
+    <row r="28" spans="1:6" ht="15.75">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75">
+    <row r="29" spans="1:6" ht="15.75">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75">
+    <row r="30" spans="1:6" ht="15.75">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75">
+    <row r="31" spans="1:6" ht="15.75">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75">
+    <row r="32" spans="1:6" ht="15.75">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2981,10 +3021,10 @@
       <c r="D353" s="2"/>
     </row>
     <row r="354" spans="1:4" ht="15.75">
-      <c r="A354" s="1"/>
-      <c r="B354" s="1"/>
-      <c r="C354" s="1"/>
-      <c r="D354" s="1"/>
+      <c r="A354" s="2"/>
+      <c r="B354" s="2"/>
+      <c r="C354" s="2"/>
+      <c r="D354" s="2"/>
     </row>
     <row r="355" spans="1:4" ht="15.75">
       <c r="A355" s="1"/>
@@ -3466,15 +3506,24 @@
       <c r="C434" s="1"/>
       <c r="D434" s="1"/>
     </row>
+    <row r="435" spans="1:4" ht="15.75">
+      <c r="A435" s="1"/>
+      <c r="B435" s="1"/>
+      <c r="C435" s="1"/>
+      <c r="D435" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="F8:F12"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
+  <mergeCells count="10">
     <mergeCell ref="B1:D2"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Phân công , tối họp :D
</commit_message>
<xml_diff>
--- a/PhanCong.xlsx
+++ b/PhanCong.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Công việc</t>
   </si>
@@ -114,22 +114,25 @@
     <t>Thứ 4 (30/11/2010)</t>
   </si>
   <si>
-    <t>Người dùng xác nhận link , báo đăng kí thành công với  2 tài khoản, đăng tin tuyển dụng.</t>
-  </si>
-  <si>
     <t>UC cập nhật thông tin cho người tìm việc với nhà tuyển dụng, update thông tin cập nhật vào csdl.</t>
   </si>
   <si>
     <t>Ngăn chặn ko cho xem subpage khi chưa đăng nhập. UC tìm kiếm dơn giản và nâng cao.</t>
   </si>
   <si>
-    <t>Đăng nhập , kiểm tra user đăng nhập thành công, upload CV , lưu CV.</t>
-  </si>
-  <si>
-    <t>FAQ (1 dạng hướng dẫn người dùng đăng kí) , hiển thị user nào đang đăng nhập.</t>
-  </si>
-  <si>
     <t>Feature đăng nhập, tìm kiếm, update thông tin, đăng tải tin tức.</t>
+  </si>
+  <si>
+    <t>hiển thị captchar từ csdl, gửi mail…</t>
+  </si>
+  <si>
+    <t>Hoàn tất feature đăng kí 2 loại tài khoản. Báo thành công đăng nhập user, hiển thị user đang đăng nhập.</t>
+  </si>
+  <si>
+    <t>FAQ (1 dạng hướng dẫn người dùng đăng kí, tạo hồ sơ). Tạo mẫu cv có sẵn.</t>
+  </si>
+  <si>
+    <t>Đăng nhập , kiểm tra user đăng nhập thành công, up và lưu CV. Gửi nhận thông tin cho nhà tuyển dụng.</t>
   </si>
 </sst>
 </file>
@@ -372,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -449,6 +452,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -458,10 +468,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -481,42 +523,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -815,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -830,20 +836,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -859,22 +865,22 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:12" ht="36" customHeight="1">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="50"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="39.75" customHeight="1">
-      <c r="B5" s="35"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -916,10 +922,10 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="64.5" customHeight="1">
-      <c r="A8" s="46">
+      <c r="A8" s="43">
         <v>1</v>
       </c>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="37" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -931,13 +937,13 @@
       <c r="E8" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="40" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="31.5">
-      <c r="A9" s="47"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="44"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="8" t="s">
         <v>5</v>
       </c>
@@ -947,11 +953,11 @@
       <c r="E9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="44"/>
+      <c r="F9" s="41"/>
     </row>
     <row r="10" spans="1:12" ht="31.5">
-      <c r="A10" s="47"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="44"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="8" t="s">
         <v>8</v>
       </c>
@@ -961,11 +967,11 @@
       <c r="E10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="44"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:12" ht="63">
-      <c r="A11" s="47"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
@@ -975,11 +981,11 @@
       <c r="E11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="44"/>
+      <c r="F11" s="41"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="A12" s="48"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
@@ -987,7 +993,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="45"/>
+      <c r="F12" s="42"/>
     </row>
     <row r="13" spans="1:12" ht="21" customHeight="1">
       <c r="A13" s="21"/>
@@ -1004,10 +1010,10 @@
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:12" ht="45" customHeight="1">
-      <c r="A15" s="40">
+      <c r="A15" s="34">
         <v>2</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="34" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="17" t="s">
@@ -1017,13 +1023,13 @@
         <v>28</v>
       </c>
       <c r="E15" s="16"/>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="40" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="33" customHeight="1">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="18" t="s">
         <v>5</v>
       </c>
@@ -1031,11 +1037,11 @@
         <v>26</v>
       </c>
       <c r="E16" s="15"/>
-      <c r="F16" s="44"/>
+      <c r="F16" s="41"/>
     </row>
     <row r="17" spans="1:6" ht="39" customHeight="1">
-      <c r="A17" s="41"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="18" t="s">
         <v>8</v>
       </c>
@@ -1043,11 +1049,11 @@
         <v>27</v>
       </c>
       <c r="E17" s="15"/>
-      <c r="F17" s="44"/>
+      <c r="F17" s="41"/>
     </row>
     <row r="18" spans="1:6" ht="34.5" customHeight="1">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="18" t="s">
         <v>6</v>
       </c>
@@ -1055,11 +1061,11 @@
         <v>24</v>
       </c>
       <c r="E18" s="15"/>
-      <c r="F18" s="44"/>
+      <c r="F18" s="41"/>
     </row>
     <row r="19" spans="1:6" ht="45.75" customHeight="1">
-      <c r="A19" s="42"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="19" t="s">
         <v>7</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>29</v>
       </c>
       <c r="E19" s="12"/>
-      <c r="F19" s="45"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="1:6" ht="15.75">
       <c r="A20" s="2"/>
@@ -1088,70 +1094,72 @@
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="36.75" customHeight="1">
-      <c r="A23" s="40">
+      <c r="A23" s="34">
         <v>3</v>
       </c>
-      <c r="B23" s="49" t="s">
-        <v>37</v>
+      <c r="B23" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="43" t="s">
+      <c r="D23" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="40" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="35.25" customHeight="1">
-      <c r="A24" s="41"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="29" t="s">
-        <v>36</v>
+      <c r="D24" s="32" t="s">
+        <v>37</v>
       </c>
       <c r="E24" s="15"/>
-      <c r="F24" s="44"/>
+      <c r="F24" s="41"/>
     </row>
     <row r="25" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A25" s="41"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="38"/>
       <c r="C25" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="29" t="s">
-        <v>33</v>
+      <c r="D25" s="28" t="s">
+        <v>32</v>
       </c>
       <c r="E25" s="15"/>
-      <c r="F25" s="44"/>
+      <c r="F25" s="41"/>
     </row>
     <row r="26" spans="1:6" ht="34.5" customHeight="1">
-      <c r="A26" s="41"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="35"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="44"/>
+      <c r="D26" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="41"/>
     </row>
     <row r="27" spans="1:6" ht="36" customHeight="1">
-      <c r="A27" s="42"/>
-      <c r="B27" s="51"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="39"/>
       <c r="C27" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="45"/>
+      <c r="D27" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="30"/>
+      <c r="F27" s="42"/>
     </row>
     <row r="28" spans="1:6" ht="15.75">
       <c r="A28" s="2"/>
@@ -3603,6 +3611,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B1:D2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="F23:F27"/>
@@ -3610,12 +3624,6 @@
     <mergeCell ref="F8:F12"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B1:D2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>